<commit_message>
- remove S201C module
prefect the communication function
</commit_message>
<xml_diff>
--- a/data/MsgFormat.xlsx
+++ b/data/MsgFormat.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\STM32\project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC01C55-8053-4419-AACB-AEC60B1E1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2AFD4F-9DC3-41DB-AD3B-3A78605BB3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +34,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Leihui Li</author>
+  </authors>
+  <commentList>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{46C48AA1-7062-478A-8C36-9B9D780D1691}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Leihui Li:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+字节</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Accelerate</t>
   </si>
@@ -136,13 +171,64 @@
   </si>
   <si>
     <t>排水口状态</t>
+  </si>
+  <si>
+    <t>水流速传感器</t>
+  </si>
+  <si>
+    <t>Size(In code)</t>
+  </si>
+  <si>
+    <t>潜艇</t>
+  </si>
+  <si>
+    <t>数据收集</t>
+  </si>
+  <si>
+    <t>数据发送</t>
+  </si>
+  <si>
+    <t>物理传输</t>
+  </si>
+  <si>
+    <t>数据开始接收</t>
+  </si>
+  <si>
+    <t>数据接收完成</t>
+  </si>
+  <si>
+    <t>发送回应报文</t>
+  </si>
+  <si>
+    <t>开始数据接收</t>
+  </si>
+  <si>
+    <t>数据接受完成</t>
+  </si>
+  <si>
+    <t>分析回应报文</t>
+  </si>
+  <si>
+    <t>消耗时间</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>对象</t>
+  </si>
+  <si>
+    <t>上位机(PC)</t>
+  </si>
+  <si>
+    <t>≈2s 最快1s 室内测试平均1.2s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +243,19 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,7 +265,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -174,20 +273,151 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -205,6 +435,174 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F86444CA-CBEC-4674-BE9C-E7FC3EC51BD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1773115" y="952500"/>
+          <a:ext cx="4066443" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>923192</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEFF0E98-A7BB-4471-BEBF-FB8C3B5F5AA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="1340827"/>
+          <a:ext cx="3414346" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>615462</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFC675AB-CBFD-4072-9D16-AD0AE41CDD21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="615462" y="1333500"/>
+          <a:ext cx="3780692" cy="7327"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,11 +867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,272 +881,331 @@
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="G2" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>16</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
         <v>32</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="G4" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
         <v>32</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+      <c r="G5" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
         <v>32</v>
       </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
         <v>32</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+      <c r="G7" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
         <v>8</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
+      <c r="G8" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
         <v>8</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="G9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
         <v>8</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="G10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+      <c r="G11" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+      <c r="G12" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
+      <c r="G13" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="G14" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <f>COUNTA(B2:B14)</f>
         <v>13</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
         <f>E2*D2 + E3*D3+SUM(E4:E14)</f>
         <v>252</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="G15">
+        <f>SUM(G4:G14)+G2*D2+G3*D3</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f>E15/8</f>
+        <v>31.5</v>
+      </c>
+      <c r="G16">
+        <f>D4</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -756,5 +1213,142 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB296EE-26EE-4CBF-9DD5-048EE1FF7375}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>